<commit_message>
added all form2400 med valueset, started R4 connection guide
</commit_message>
<xml_diff>
--- a/docs/ValueSet-med-cyclophosphamide-vs.xlsx
+++ b/docs/ValueSet-med-cyclophosphamide-vs.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="109">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-07-29T16:31:05-05:00</t>
+    <t>2022-08-02T11:06:34-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -109,9 +109,6 @@
   </si>
   <si>
     <t>Endoxana</t>
-  </si>
-  <si>
-    <t>CC0010583</t>
   </si>
   <si>
     <t>1545988</t>
@@ -607,7 +604,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B44"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -654,300 +651,300 @@
         <v>32</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="2">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="2">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="2">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="2">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="2">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="2">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="2">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="2">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B42" t="s" s="2">
         <v>106</v>
@@ -958,15 +955,7 @@
         <v>107</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="s" s="2">
         <v>108</v>
-      </c>
-      <c r="B44" t="s" s="2">
-        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>